<commit_message>
Updated kernel and for docs and gh-pages.
</commit_message>
<xml_diff>
--- a/docs/tutorials/intro-series/Audit-AddABC.xlsx
+++ b/docs/tutorials/intro-series/Audit-AddABC.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instantiation" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="_add_a_b" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="_add_ab_c" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="__footings__" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="Main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Instantiation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="_add_a_b" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="_add_ab_c" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Output" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="__footings__" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -43,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,14 +51,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -457,7 +458,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AddABC(*, a: int, b: int, c: int) -&gt; 'AddABC'</t>
+          <t>AddABC(*, a: int, b: int, c: int)</t>
         </is>
       </c>
     </row>
@@ -762,7 +763,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[parameter.a, parameter.b]</t>
+          <t>(parameter.a, parameter.b)</t>
         </is>
       </c>
     </row>
@@ -775,7 +776,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[intermediate.ab]</t>
+          <t>(intermediate.ab,)</t>
         </is>
       </c>
     </row>
@@ -881,7 +882,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[intermediate.ab, parameter.c]</t>
+          <t>(intermediate.ab, parameter.c)</t>
         </is>
       </c>
     </row>
@@ -894,7 +895,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[return.abc]</t>
+          <t>(return.abc,)</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1986,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[parameter.a]</t>
+          <t>/parameter.a/</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2024,7 +2025,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>[parameter.a]</t>
+          <t>/parameter.a/</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2063,7 +2064,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[parameter.b]</t>
+          <t>/parameter.b/</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2102,7 +2103,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[parameter.b]</t>
+          <t>/parameter.b/</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2141,7 +2142,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[parameter.c]</t>
+          <t>/parameter.c/</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2180,7 +2181,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[parameter.c]</t>
+          <t>/parameter.c/</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2596,7 +2597,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>[intermediate.ab]</t>
+          <t>/intermediate.ab/</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2635,7 +2636,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>[intermediate.ab]</t>
+          <t>/intermediate.ab/</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3051,7 +3052,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[return.abc]</t>
+          <t>/return.abc/</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3090,7 +3091,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>[return.abc]</t>
+          <t>/return.abc/</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3158,7 +3159,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>[abc]</t>
+          <t>/abc/</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3197,7 +3198,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[abc]</t>
+          <t>/abc/</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">

</xml_diff>